<commit_message>
audp role and permission change for production3
</commit_message>
<xml_diff>
--- a/role_permission_files/production3_role_permission_v0.5.xlsx
+++ b/role_permission_files/production3_role_permission_v0.5.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="7050" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="7050" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="version" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="183">
   <si>
     <t>Version Control</t>
   </si>
@@ -436,36 +436,15 @@
     <t>jackpot_meter</t>
   </si>
   <si>
-    <t>list_reset_game_meter</t>
-  </si>
-  <si>
-    <t>reset_game</t>
-  </si>
-  <si>
     <t>reset_game_meter</t>
   </si>
   <si>
-    <t>reset_terminal</t>
-  </si>
-  <si>
-    <t>log</t>
-  </si>
-  <si>
-    <t>reset_gaming_meter_log</t>
-  </si>
-  <si>
-    <t>list_reset_jackpot_meter</t>
-  </si>
-  <si>
     <t>reset</t>
   </si>
   <si>
     <t>reset_jackpot_meter</t>
   </si>
   <si>
-    <t>reset_jackpot_meter_log</t>
-  </si>
-  <si>
     <t>lock</t>
   </si>
   <si>
@@ -601,7 +580,10 @@
     <t>v0.5</t>
   </si>
   <si>
-    <t>add Cage "addcredit" to Y:5000</t>
+    <t>add Cage "addcredit" to Y:5000, corrected permission name for AUDP</t>
+  </si>
+  <si>
+    <t>reset_terminal_game_meter</t>
   </si>
 </sst>
 </file>
@@ -1166,7 +1148,7 @@
         <v>31</v>
       </c>
       <c r="F5" s="43" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="I5" s="38" t="s">
         <v>26</v>
@@ -1174,7 +1156,7 @@
     </row>
     <row r="6" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C6" s="35" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="D6" s="36">
         <v>42900</v>
@@ -1183,35 +1165,35 @@
         <v>31</v>
       </c>
       <c r="F6" s="43" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C7" s="35" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="D7" s="36">
         <v>42913</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="F7" s="43" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C8" s="35" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="D8" s="36">
         <v>42914</v>
       </c>
       <c r="E8" s="35" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="F8" s="43" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.25">
@@ -1967,7 +1949,7 @@
         <v>44</v>
       </c>
       <c r="L2" s="23" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -4405,11 +4387,11 @@
   </sheetPr>
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4613,7 +4595,7 @@
         <v>134</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>24</v>
@@ -4629,10 +4611,10 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="E9" s="24" t="s">
         <v>24</v>
@@ -4648,10 +4630,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>137</v>
+        <v>13</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>24</v>
@@ -4674,7 +4656,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>24</v>
@@ -4694,10 +4676,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>24</v>
@@ -4714,7 +4696,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>24</v>
@@ -4742,7 +4724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -4802,7 +4784,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>90</v>
@@ -4810,7 +4792,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>90</v>
@@ -4824,7 +4806,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>90</v>
@@ -4847,7 +4829,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>90</v>
@@ -4861,7 +4843,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>90</v>
@@ -4884,10 +4866,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>24</v>
@@ -4895,10 +4877,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>24</v>
@@ -4906,21 +4888,21 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>24</v>
@@ -4928,10 +4910,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>24</v>
@@ -4939,10 +4921,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>24</v>
@@ -4962,10 +4944,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>24</v>
@@ -4976,7 +4958,7 @@
         <v>52</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>24</v>
@@ -4984,10 +4966,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>24</v>
@@ -4995,10 +4977,10 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>24</v>
@@ -5006,10 +4988,10 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>24</v>
@@ -5029,10 +5011,10 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>24</v>
@@ -5040,10 +5022,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>24</v>
@@ -5051,7 +5033,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>9</v>
@@ -5062,10 +5044,10 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>24</v>
@@ -5079,10 +5061,10 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>24</v>
@@ -5124,10 +5106,10 @@
         <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="D1" s="2">
         <v>1</v>
@@ -5144,7 +5126,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="D2" s="26" t="s">
         <v>40</v>
@@ -5158,10 +5140,10 @@
         <v>11</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D3" s="29"/>
       <c r="E3" s="29"/>
@@ -5171,23 +5153,23 @@
         <v>99</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D4" s="29"/>
       <c r="E4" s="29"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D5" s="29"/>
       <c r="E5" s="29"/>
@@ -5197,10 +5179,10 @@
         <v>106</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D6" s="29"/>
       <c r="E6" s="29"/>
@@ -5210,10 +5192,10 @@
         <v>11</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D7" s="29"/>
       <c r="E7" s="29"/>
@@ -5223,23 +5205,23 @@
         <v>99</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D8" s="29"/>
       <c r="E8" s="29"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D9" s="29"/>
       <c r="E9" s="29"/>
@@ -5249,10 +5231,10 @@
         <v>106</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D10" s="29"/>
       <c r="E10" s="29"/>
@@ -5262,10 +5244,10 @@
         <v>11</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D11" s="29"/>
       <c r="E11" s="29"/>
@@ -5275,23 +5257,23 @@
         <v>99</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D12" s="29"/>
       <c r="E12" s="29"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D13" s="29"/>
       <c r="E13" s="29"/>
@@ -5301,10 +5283,10 @@
         <v>106</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D14" s="29"/>
       <c r="E14" s="29"/>
@@ -5317,7 +5299,7 @@
         <v>88</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D15" s="29"/>
       <c r="E15" s="29"/>
@@ -5330,20 +5312,20 @@
         <v>88</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D16" s="29"/>
       <c r="E16" s="29"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B17" s="28" t="s">
         <v>88</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D17" s="29"/>
       <c r="E17" s="29"/>
@@ -5356,7 +5338,7 @@
         <v>88</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D18" s="29"/>
       <c r="E18" s="29"/>
@@ -5366,16 +5348,16 @@
         <v>11</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -5383,33 +5365,33 @@
         <v>99</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -5417,16 +5399,16 @@
         <v>106</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -5434,10 +5416,10 @@
         <v>11</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D23" s="29"/>
       <c r="E23" s="29"/>
@@ -5447,23 +5429,23 @@
         <v>99</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D24" s="29"/>
       <c r="E24" s="29"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D25" s="29"/>
       <c r="E25" s="29"/>
@@ -5473,10 +5455,10 @@
         <v>106</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D26" s="29"/>
       <c r="E26" s="29"/>
@@ -5486,10 +5468,10 @@
         <v>11</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D27" s="29"/>
       <c r="E27" s="29"/>
@@ -5499,23 +5481,23 @@
         <v>99</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D28" s="29"/>
       <c r="E28" s="29"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B29" s="28" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D29" s="29"/>
       <c r="E29" s="29"/>
@@ -5525,10 +5507,10 @@
         <v>106</v>
       </c>
       <c r="B30" s="28" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D30" s="29"/>
       <c r="E30" s="29"/>
@@ -5538,10 +5520,10 @@
         <v>11</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D31" s="29"/>
       <c r="E31" s="29"/>
@@ -5551,23 +5533,23 @@
         <v>99</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D32" s="29"/>
       <c r="E32" s="29"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B33" s="28" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D33" s="29"/>
       <c r="E33" s="29"/>
@@ -5577,10 +5559,10 @@
         <v>106</v>
       </c>
       <c r="B34" s="28" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D34" s="29"/>
       <c r="E34" s="29"/>
@@ -5590,10 +5572,10 @@
         <v>11</v>
       </c>
       <c r="B35" s="28" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D35" s="29"/>
       <c r="E35" s="29"/>
@@ -5603,23 +5585,23 @@
         <v>99</v>
       </c>
       <c r="B36" s="28" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D36" s="29"/>
       <c r="E36" s="29"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B37" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="B37" s="28" t="s">
-        <v>178</v>
-      </c>
       <c r="C37" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D37" s="29"/>
       <c r="E37" s="29"/>
@@ -5629,10 +5611,10 @@
         <v>106</v>
       </c>
       <c r="B38" s="28" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D38" s="29"/>
       <c r="E38" s="29"/>

</xml_diff>